<commit_message>
stack and queue dsa lab da
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1646,11 +1646,11 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A342" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D364" activeCellId="0" sqref="D364"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A303" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C317" activeCellId="0" sqref="C317"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.33984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -5002,7 +5002,7 @@
         <v>311</v>
       </c>
       <c r="C317" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
krushkal and hash fucntion added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1649,8 +1649,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C370" activeCellId="0" sqref="C370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5560,7 +5560,7 @@
         <v>363</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>